<commit_message>
rotate added new video
</commit_message>
<xml_diff>
--- a/pypf/data/attn_example_rev.xlsx
+++ b/pypf/data/attn_example_rev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schva\Prog\py_proj\pypf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFECDCC-E432-4AB4-AD2E-068CDABACAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64477F34-EF1C-4CAC-9182-4EA729976C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22635" yWindow="810" windowWidth="19230" windowHeight="14670" xr2:uid="{8DCF90F5-8D2C-4BA0-8AE6-5C94FE878D20}"/>
   </bookViews>
@@ -928,7 +928,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +997,7 @@
         <v>836</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>967</v>
@@ -1260,7 +1260,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>848</v>

</xml_diff>